<commit_message>
Notifications and Chat tests
</commit_message>
<xml_diff>
--- a/MarsQA-1/NunitTests/Data/TestData.xlsx
+++ b/MarsQA-1/NunitTests/Data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\MarsProject_Specflow\SpecflowSourceMRS\MarsQA-1\SpecflowTests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AdvancedTask\MarsQA-1\NunitTests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AD1A77-D8C4-4C28-A0B7-255282CCBECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98995AD-288D-4689-9D97-CF1AFBBF2A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2640" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="119">
   <si>
     <t>FirstName</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>Patel</t>
+  </si>
+  <si>
+    <t>bmacedo1987@gmail.com</t>
+  </si>
+  <si>
+    <t>industryconnect</t>
+  </si>
+  <si>
+    <t>johndoe@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -445,6 +454,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -475,7 +491,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,8 +501,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -508,10 +525,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -896,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1040,9 +1059,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1105,7 +1126,27 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{2B4F0894-2020-4903-BF14-B8A005C127EA}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{6B716EE0-00E7-4477-9674-EA1FCA3E14E7}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>